<commit_message>
Uppdaterad brief, frågor och use case ritning
</commit_message>
<xml_diff>
--- a/Brief1.xlsx
+++ b/Brief1.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maja\Desktop\ProjectPetra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joel\Desktop\ProjectPetra\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7995"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7155" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Blad2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="68">
   <si>
     <t>Snabb översikt över produktionen</t>
   </si>
@@ -132,13 +133,109 @@
   </si>
   <si>
     <t>Se planering för 1-2mån framåt</t>
+  </si>
+  <si>
+    <t>Backlog items</t>
+  </si>
+  <si>
+    <t>Item number</t>
+  </si>
+  <si>
+    <t>Item</t>
+  </si>
+  <si>
+    <t>Estimated time</t>
+  </si>
+  <si>
+    <t>Priority</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>ToDo</t>
+  </si>
+  <si>
+    <t>Köra med en test implementering av Identity med Google</t>
+  </si>
+  <si>
+    <t>Test Identity</t>
+  </si>
+  <si>
+    <t>Implementera Identity</t>
+  </si>
+  <si>
+    <t>Implementera Identity, få igång alla funktioner</t>
+  </si>
+  <si>
+    <t>Modulera Databas</t>
+  </si>
+  <si>
+    <t>Finslipa, modulera slutgiltlig databas</t>
+  </si>
+  <si>
+    <t>Implementera rest databas</t>
+  </si>
+  <si>
+    <t>Implementering av resterande databas med entity framework code first</t>
+  </si>
+  <si>
+    <t>Layout login-sida</t>
+  </si>
+  <si>
+    <t>Styla login sidan med Material Design</t>
+  </si>
+  <si>
+    <t>Implementera wep-api</t>
+  </si>
+  <si>
+    <t>Implementer api/service för alla klasser/tabeller, och dess respektive angular</t>
+  </si>
+  <si>
+    <t>Implementering av MaterDes</t>
+  </si>
+  <si>
+    <t>Implementer resterande design, Material Design</t>
+  </si>
+  <si>
+    <t>Skriva testcases</t>
+  </si>
+  <si>
+    <t>Skriva testcases för sidan</t>
+  </si>
+  <si>
+    <t>Köra igenom testcases</t>
+  </si>
+  <si>
+    <t>Köra igenom alla testcases för sidan</t>
+  </si>
+  <si>
+    <t>Fixa till eventuella fel</t>
+  </si>
+  <si>
+    <t>Rätta till alla eventuella fel som vi har upptäckt</t>
+  </si>
+  <si>
+    <t>Implenetera loggning av fel</t>
+  </si>
+  <si>
+    <t>Implementera funktion som loggar alla fel och exceptions</t>
+  </si>
+  <si>
+    <t>Implementera div funktioner</t>
+  </si>
+  <si>
+    <t>Implementering av diverse funktioner, features</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -166,8 +263,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="17">
+  <fills count="18">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -257,6 +369,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFB17ED8"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
   </fills>
@@ -321,7 +438,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -333,8 +450,9 @@
     <xf numFmtId="0" fontId="1" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="4" xfId="2" applyBorder="1"/>
@@ -358,13 +476,16 @@
     <xf numFmtId="0" fontId="2" fillId="13" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="15" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="16" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" xfId="11"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="12">
     <cellStyle name="40% - Dekorfärg1" xfId="2" builtinId="31"/>
     <cellStyle name="40% - Dekorfärg2" xfId="4" builtinId="35"/>
     <cellStyle name="40% - Dekorfärg3" xfId="6" builtinId="39"/>
     <cellStyle name="40% - Dekorfärg4" xfId="8" builtinId="43"/>
     <cellStyle name="40% - Dekorfärg6" xfId="10" builtinId="51"/>
+    <cellStyle name="Bra" xfId="11" builtinId="26"/>
     <cellStyle name="Dekorfärg1" xfId="1" builtinId="29"/>
     <cellStyle name="Dekorfärg2" xfId="3" builtinId="33"/>
     <cellStyle name="Dekorfärg3" xfId="5" builtinId="37"/>
@@ -794,8 +915,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:J30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D25" sqref="D25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N10" sqref="N10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -974,4 +1095,295 @@
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.28515625" customWidth="1"/>
+    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" customWidth="1"/>
+    <col min="6" max="6" width="11.85546875" customWidth="1"/>
+    <col min="7" max="7" width="71.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A1" s="23" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="24"/>
+      <c r="B3" s="24" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" s="24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D3" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="F3" s="24" t="s">
+        <v>41</v>
+      </c>
+      <c r="G3" s="24" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4" t="s">
+        <v>43</v>
+      </c>
+      <c r="G4" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5">
+        <v>4</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>48</v>
+      </c>
+      <c r="D6">
+        <v>2</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G6" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>50</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+      <c r="F7" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8">
+        <v>4</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="F8" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" t="s">
+        <v>54</v>
+      </c>
+      <c r="D9">
+        <v>6</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10">
+        <v>4</v>
+      </c>
+      <c r="E10">
+        <v>1</v>
+      </c>
+      <c r="F10" t="s">
+        <v>43</v>
+      </c>
+      <c r="G10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" t="s">
+        <v>56</v>
+      </c>
+      <c r="D11">
+        <v>8</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
+      </c>
+      <c r="F11" t="s">
+        <v>43</v>
+      </c>
+      <c r="G11" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12" t="s">
+        <v>58</v>
+      </c>
+      <c r="D12">
+        <v>2</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="F12" t="s">
+        <v>43</v>
+      </c>
+      <c r="G12" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>2</v>
+      </c>
+      <c r="F13" t="s">
+        <v>43</v>
+      </c>
+      <c r="G13" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>62</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
+        <v>2</v>
+      </c>
+      <c r="F14" t="s">
+        <v>43</v>
+      </c>
+      <c r="G14" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15" t="s">
+        <v>64</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="F15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" t="s">
+        <v>65</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Uppdaterat estimering av projektet
</commit_message>
<xml_diff>
--- a/Brief1.xlsx
+++ b/Brief1.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="57">
   <si>
     <t>Snabb översikt över produktionen</t>
   </si>
@@ -168,9 +168,6 @@
     <t>Implementera Identity</t>
   </si>
   <si>
-    <t>Implementera Identity, få igång alla funktioner</t>
-  </si>
-  <si>
     <t>Modulera Databas</t>
   </si>
   <si>
@@ -183,52 +180,22 @@
     <t>Implementering av resterande databas med entity framework code first</t>
   </si>
   <si>
-    <t>Layout login-sida</t>
-  </si>
-  <si>
-    <t>Styla login sidan med Material Design</t>
-  </si>
-  <si>
-    <t>Implementera wep-api</t>
-  </si>
-  <si>
-    <t>Implementer api/service för alla klasser/tabeller, och dess respektive angular</t>
-  </si>
-  <si>
-    <t>Implementering av MaterDes</t>
-  </si>
-  <si>
-    <t>Implementer resterande design, Material Design</t>
-  </si>
-  <si>
-    <t>Skriva testcases</t>
-  </si>
-  <si>
-    <t>Skriva testcases för sidan</t>
-  </si>
-  <si>
-    <t>Köra igenom testcases</t>
-  </si>
-  <si>
-    <t>Köra igenom alla testcases för sidan</t>
-  </si>
-  <si>
-    <t>Fixa till eventuella fel</t>
-  </si>
-  <si>
-    <t>Rätta till alla eventuella fel som vi har upptäckt</t>
-  </si>
-  <si>
-    <t>Implenetera loggning av fel</t>
-  </si>
-  <si>
-    <t>Implementera funktion som loggar alla fel och exceptions</t>
-  </si>
-  <si>
-    <t>Implementera div funktioner</t>
-  </si>
-  <si>
-    <t>Implementering av diverse funktioner, features</t>
+    <t>Lägga till alla dess respektive funktioner</t>
+  </si>
+  <si>
+    <t>Implementera ToDo</t>
+  </si>
+  <si>
+    <t>Implementera Identity, få igång alla funktioner, plus layout</t>
+  </si>
+  <si>
+    <t>Layout för login-sida</t>
+  </si>
+  <si>
+    <t>Implementera all layout för login sida och dess respektive partial views</t>
+  </si>
+  <si>
+    <t>…</t>
   </si>
 </sst>
 </file>
@@ -1099,10 +1066,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1113,7 +1080,8 @@
     <col min="4" max="4" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="9.85546875" customWidth="1"/>
     <col min="6" max="6" width="11.85546875" customWidth="1"/>
-    <col min="7" max="7" width="71.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="66.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="38" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
@@ -1179,7 +1147,7 @@
         <v>43</v>
       </c>
       <c r="G5" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1187,7 +1155,7 @@
         <v>3</v>
       </c>
       <c r="C6" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="D6">
         <v>2</v>
@@ -1199,15 +1167,15 @@
         <v>43</v>
       </c>
       <c r="G6" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B7">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="D7">
         <v>2</v>
@@ -1219,18 +1187,18 @@
         <v>43</v>
       </c>
       <c r="G7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B8">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="D8">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="E8">
         <v>1</v>
@@ -1239,7 +1207,7 @@
         <v>43</v>
       </c>
       <c r="G8" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1247,10 +1215,10 @@
         <v>6</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D9">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -1259,7 +1227,7 @@
         <v>43</v>
       </c>
       <c r="G9" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1267,119 +1235,7 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>66</v>
-      </c>
-      <c r="D10">
-        <v>4</v>
-      </c>
-      <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B11">
-        <v>8</v>
-      </c>
-      <c r="C11" t="s">
         <v>56</v>
-      </c>
-      <c r="D11">
-        <v>8</v>
-      </c>
-      <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11" t="s">
-        <v>43</v>
-      </c>
-      <c r="G11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B12">
-        <v>9</v>
-      </c>
-      <c r="C12" t="s">
-        <v>58</v>
-      </c>
-      <c r="D12">
-        <v>2</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-      <c r="F12" t="s">
-        <v>43</v>
-      </c>
-      <c r="G12" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B13">
-        <v>10</v>
-      </c>
-      <c r="C13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13">
-        <v>2</v>
-      </c>
-      <c r="E13">
-        <v>2</v>
-      </c>
-      <c r="F13" t="s">
-        <v>43</v>
-      </c>
-      <c r="G13" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B14">
-        <v>11</v>
-      </c>
-      <c r="C14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D14">
-        <v>2</v>
-      </c>
-      <c r="E14">
-        <v>2</v>
-      </c>
-      <c r="F14" t="s">
-        <v>43</v>
-      </c>
-      <c r="G14" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="B15">
-        <v>12</v>
-      </c>
-      <c r="C15" t="s">
-        <v>64</v>
-      </c>
-      <c r="D15">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>3</v>
-      </c>
-      <c r="F15" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" t="s">
-        <v>65</v>
       </c>
     </row>
   </sheetData>

</xml_diff>